<commit_message>
add more to the guide
</commit_message>
<xml_diff>
--- a/how to navigate.xlsx
+++ b/how to navigate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\xampp\htdocs\Nhom420\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B2C50E-9E1D-4F3C-A4BA-637552F61977}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D95651-A915-407B-A60D-A8D864DB1533}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>url</t>
   </si>
@@ -102,7 +102,25 @@
     <t>Đổ hết dữ liệu từ mục sản phẩm lên màn hình</t>
   </si>
   <si>
-    <t>Chưa Hoàn Thành</t>
+    <t>Nhom420/Login</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Hiện màn hình login</t>
+  </si>
+  <si>
+    <t>Chưa</t>
+  </si>
+  <si>
+    <t>Nhom420/Register</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Hiện màn hình đăng kí</t>
   </si>
 </sst>
 </file>
@@ -420,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +520,7 @@
         <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -515,11 +533,11 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" t="s">
         <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -532,11 +550,11 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
       <c r="E6" t="s">
         <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -554,6 +572,43 @@
       </c>
       <c r="E7" t="s">
         <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>